<commit_message>
add test sql and import
</commit_message>
<xml_diff>
--- a/documents/example.xlsx
+++ b/documents/example.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T127"/>
+  <dimension ref="A1:T128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15608</v>
+        <v>37267</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -548,13 +548,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>43383.73309027778</v>
+        <v>43775.65305555556</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>35848</v>
+        <v>78258</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -630,30 +630,30 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E3" t="n">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>43770.74552083333</v>
+        <v>43886.55609953704</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>36216</v>
+        <v>98923</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -712,30 +712,30 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="E4" t="n">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>43773.51679398148</v>
+        <v>43941.60271990741</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>56349</v>
+        <v>17180</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="E5" t="n">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>43815.63793981481</v>
+        <v>43385.71641203704</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>18362</v>
+        <v>17134</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -868,7 +868,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>77229</v>
+        <v>58474</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -876,30 +876,30 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E6" t="n">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>43882.60393518519</v>
+        <v>43819.65837962963</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -950,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>97943</v>
+        <v>120633</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="E7" t="n">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>43938.57678240741</v>
+        <v>44012.81336805555</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>118690</v>
+        <v>38513</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1040,30 +1040,30 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="E8" t="n">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>44005.76278935185</v>
+        <v>43777.64254629629</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1114,7 +1114,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>57477</v>
+        <v>59267</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>43817.69225694444</v>
+        <v>43822.89885416667</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1196,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>119680</v>
+        <v>79436</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1204,13 +1204,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="E10" t="n">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>44008.61280092593</v>
+        <v>43887.62052083333</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>37267</v>
+        <v>99934</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1286,30 +1286,30 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="E11" t="n">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>43775.65305555556</v>
+        <v>43943.62464120371</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1360,7 +1360,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>78258</v>
+        <v>121184</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="E12" t="n">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>43886.55609953704</v>
+        <v>44013.52458333333</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>98923</v>
+        <v>60190</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1450,30 +1450,30 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="E13" t="n">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>43941.60271990741</v>
+        <v>43824.68055555555</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1524,7 +1524,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>17180</v>
+        <v>80514</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1532,30 +1532,30 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>43385.71641203704</v>
+        <v>43889.66643518519</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>17134</v>
+        <v>18363</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1606,7 +1606,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>58474</v>
+        <v>100889</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1614,30 +1614,30 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="E15" t="n">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>43819.65837962963</v>
+        <v>43945.61356481481</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1688,7 +1688,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>120633</v>
+        <v>39673</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1696,30 +1696,30 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="E16" t="n">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>44012.81336805555</v>
+        <v>43780.68399305556</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1770,7 +1770,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>38513</v>
+        <v>101758</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1778,30 +1778,30 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="E17" t="n">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>43777.64254629629</v>
+        <v>43949.73225694444</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1852,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>59267</v>
+        <v>122539</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1860,30 +1860,30 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="E18" t="n">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>43822.89885416667</v>
+        <v>44035.80074074074</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>18362</v>
+        <v>19041</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1934,7 +1934,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>79436</v>
+        <v>122736</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1942,13 +1942,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E19" t="n">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>43887.62052083333</v>
+        <v>44035.84535879629</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1961,7 +1961,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2016,7 +2016,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>99934</v>
+        <v>40809</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -2024,30 +2024,30 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="E20" t="n">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>43943.62464120371</v>
+        <v>43782.66458333333</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2098,7 +2098,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>121184</v>
+        <v>61154</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -2106,30 +2106,30 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="E21" t="n">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>44013.52458333333</v>
+        <v>43826.62660879629</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2180,7 +2180,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>39673</v>
+        <v>81404</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -2188,30 +2188,30 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="E22" t="n">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>43780.68399305556</v>
+        <v>43893.36340277778</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2262,7 +2262,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>80514</v>
+        <v>123491</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -2270,13 +2270,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="E23" t="n">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>43889.66643518519</v>
+        <v>44036.95002314815</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -2289,7 +2289,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2344,7 +2344,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>100889</v>
+        <v>20412</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -2352,30 +2352,30 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="E24" t="n">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>43945.61356481481</v>
+        <v>43727.69207175926</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2426,7 +2426,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>60190</v>
+        <v>61789</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2434,13 +2434,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E25" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>43824.68055555555</v>
+        <v>43829.57429398148</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2508,7 +2508,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>101758</v>
+        <v>82522</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -2516,17 +2516,17 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E26" t="n">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>43949.73225694444</v>
+        <v>43894.65866898148</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2590,7 +2590,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>122539</v>
+        <v>102567</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -2598,13 +2598,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E27" t="n">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>44035.80074074074</v>
+        <v>43950.60326388889</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -2617,7 +2617,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>19041</v>
+        <v>18363</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2672,7 +2672,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>122736</v>
+        <v>42003</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -2680,30 +2680,30 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="E28" t="n">
-        <v>143</v>
+        <v>54</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>44035.84535879629</v>
+        <v>43784.65104166666</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2754,7 +2754,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>40809</v>
+        <v>103223</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -2762,13 +2762,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="E29" t="n">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>43782.66458333333</v>
+        <v>43952.52496527778</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -2777,15 +2777,15 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2836,7 +2836,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>61154</v>
+        <v>124423</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -2844,30 +2844,30 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E30" t="n">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>43826.62660879629</v>
+        <v>44039.59793981481</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>18362</v>
+        <v>19041</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2918,7 +2918,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>81404</v>
+        <v>21582</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -2926,30 +2926,30 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="E31" t="n">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>43893.36340277778</v>
+        <v>43728.67512731482</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3000,7 +3000,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>123491</v>
+        <v>62788</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -3008,30 +3008,30 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="E32" t="n">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>44036.95002314815</v>
+        <v>43840.66684027778</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3082,7 +3082,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20412</v>
+        <v>83468</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -3090,30 +3090,30 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="E33" t="n">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>43727.69207175926</v>
+        <v>43896.60649305556</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3164,7 +3164,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>61789</v>
+        <v>103818</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -3172,13 +3172,13 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="E34" t="n">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>43829.57429398148</v>
+        <v>43955.53047453704</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -3187,15 +3187,15 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3246,7 +3246,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>82522</v>
+        <v>43097</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -3254,13 +3254,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="E35" t="n">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>43894.65866898148</v>
+        <v>43787.6521412037</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -3269,15 +3269,15 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3328,7 +3328,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>102567</v>
+        <v>63704</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -3336,30 +3336,30 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E36" t="n">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>43950.60326388889</v>
+        <v>43843.68778935185</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3410,7 +3410,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>42003</v>
+        <v>83873</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -3418,30 +3418,30 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E37" t="n">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>43784.65104166666</v>
+        <v>43899.50091435185</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3492,7 +3492,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>103223</v>
+        <v>104882</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -3500,13 +3500,13 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E38" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>43952.52496527778</v>
+        <v>43962.52354166667</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -3574,7 +3574,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>124423</v>
+        <v>125653</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -3582,13 +3582,13 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E39" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>44039.59793981481</v>
+        <v>44042.78915509259</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -3738,7 +3738,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>21582</v>
+        <v>22799</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -3746,13 +3746,13 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>43728.67512731482</v>
+        <v>43731.6600925926</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -3820,7 +3820,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>62788</v>
+        <v>84647</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -3828,13 +3828,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="E42" t="n">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>43840.66684027778</v>
+        <v>43901.76452546296</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -3843,15 +3843,15 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3902,7 +3902,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>83468</v>
+        <v>106641</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -3910,13 +3910,13 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="E43" t="n">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>43896.60649305556</v>
+        <v>43966.80267361111</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -3984,7 +3984,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>103818</v>
+        <v>126649</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -3992,17 +3992,17 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="E44" t="n">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>43955.53047453704</v>
+        <v>44043.60726851852</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -4011,7 +4011,7 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4066,7 +4066,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>43097</v>
+        <v>2654</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -4074,13 +4074,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E45" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>43787.6521412037</v>
+        <v>43364.72274305556</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>18362</v>
+        <v>17134</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4148,7 +4148,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>63704</v>
+        <v>65914</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -4156,13 +4156,13 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E46" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>43843.68778935185</v>
+        <v>43847.62140046297</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4230,7 +4230,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>83873</v>
+        <v>85516</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -4238,13 +4238,13 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E47" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>43899.50091435185</v>
+        <v>43903.61269675926</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>104882</v>
+        <v>44281</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -4320,13 +4320,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="E48" t="n">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>43962.52354166667</v>
+        <v>43789.65173611111</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -4335,15 +4335,15 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4394,7 +4394,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>125653</v>
+        <v>64812</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -4402,30 +4402,30 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="E49" t="n">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>44042.78915509259</v>
+        <v>43845.63582175926</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4476,7 +4476,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>22799</v>
+        <v>107721</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -4484,13 +4484,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="E50" t="n">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>43731.6600925926</v>
+        <v>43970.54037037037</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -4499,15 +4499,15 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4558,7 +4558,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>84647</v>
+        <v>127841</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -4566,17 +4566,17 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="E51" t="n">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>43901.76452546296</v>
+        <v>44048.52226851852</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4585,7 +4585,7 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4640,7 +4640,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>106641</v>
+        <v>24747</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -4648,30 +4648,30 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="E52" t="n">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>43966.80267361111</v>
+        <v>43733.68975694444</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4722,7 +4722,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>126649</v>
+        <v>45437</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -4730,30 +4730,30 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="E53" t="n">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>44043.60726851852</v>
+        <v>43791.66946759259</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4804,7 +4804,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>44281</v>
+        <v>86471</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -4812,30 +4812,30 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="E54" t="n">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>43789.65173611111</v>
+        <v>43906.65935185185</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4886,7 +4886,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>64812</v>
+        <v>4127</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -4894,13 +4894,13 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="E55" t="n">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>43845.63582175926</v>
+        <v>43367.8046875</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -4913,7 +4913,7 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>18362</v>
+        <v>17134</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4968,7 +4968,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>85516</v>
+        <v>46563</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -4976,30 +4976,30 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E56" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>43903.61269675926</v>
+        <v>43794.64587962963</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -5050,7 +5050,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>2654</v>
+        <v>66959</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -5058,13 +5058,13 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>43364.72274305556</v>
+        <v>43850.64351851852</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -5077,7 +5077,7 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -5132,7 +5132,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>65914</v>
+        <v>87420</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -5140,30 +5140,30 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E58" t="n">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>43847.62140046297</v>
+        <v>43908.61956018519</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -5214,7 +5214,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>107721</v>
+        <v>108774</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -5222,17 +5222,17 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E59" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>43970.54037037037</v>
+        <v>43972.81844907408</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -5296,7 +5296,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>127841</v>
+        <v>129086</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -5304,13 +5304,13 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E60" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>44048.52226851852</v>
+        <v>44050.68134259259</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>24747</v>
+        <v>26631</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -5386,13 +5386,13 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E61" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>43733.68975694444</v>
+        <v>43735.91130787037</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -5460,7 +5460,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>45437</v>
+        <v>109793</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -5468,30 +5468,30 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="E62" t="n">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>43791.66946759259</v>
+        <v>43973.68603009259</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5542,7 +5542,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>86471</v>
+        <v>5598</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -5550,30 +5550,30 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>43906.65935185185</v>
+        <v>43369.90766203704</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>18363</v>
+        <v>17134</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5624,7 +5624,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>4127</v>
+        <v>47767</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -5632,13 +5632,13 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>43367.8046875</v>
+        <v>43796.65939814815</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -5651,7 +5651,7 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5706,7 +5706,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>46563</v>
+        <v>68028</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -5714,13 +5714,13 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E65" t="n">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F65" s="2" t="n">
-        <v>43794.64587962963</v>
+        <v>43852.64082175926</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -5788,7 +5788,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>66959</v>
+        <v>88470</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -5796,30 +5796,30 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E66" t="n">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>43850.64351851852</v>
+        <v>43910.624375</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5870,7 +5870,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>87420</v>
+        <v>129987</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -5878,13 +5878,13 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="E67" t="n">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>43908.61956018519</v>
+        <v>44054.73262731481</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -5897,7 +5897,7 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -5952,7 +5952,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>108774</v>
+        <v>27751</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -5960,30 +5960,30 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="E68" t="n">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>43972.81844907408</v>
+        <v>43738.68260416666</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -6034,7 +6034,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>129086</v>
+        <v>89395</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -6042,13 +6042,13 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="E69" t="n">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>44050.68134259259</v>
+        <v>43913.60846064815</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -6061,7 +6061,7 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>19041</v>
+        <v>18363</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -6116,7 +6116,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>26631</v>
+        <v>111048</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -6124,30 +6124,30 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="E70" t="n">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>43735.91130787037</v>
+        <v>43981.00342592593</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I70" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -6198,7 +6198,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>109793</v>
+        <v>7029</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -6206,30 +6206,30 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="E71" t="n">
-        <v>129</v>
+        <v>5</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>43973.68603009259</v>
+        <v>43372.33032407407</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>18363</v>
+        <v>17134</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -6280,7 +6280,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>5598</v>
+        <v>48928</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -6288,13 +6288,13 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>43369.90766203704</v>
+        <v>43798.66496527778</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="I72" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -6362,7 +6362,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>47767</v>
+        <v>69122</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="E73" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>43796.65939814815</v>
+        <v>43854.62575231482</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -6444,7 +6444,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>68028</v>
+        <v>131030</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -6452,30 +6452,30 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="E74" t="n">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>43852.64082175926</v>
+        <v>44055.63931712963</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>18362</v>
+        <v>19041</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6526,7 +6526,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>88470</v>
+        <v>28961</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -6534,30 +6534,30 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="E75" t="n">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>43910.624375</v>
+        <v>43740.68269675926</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6608,7 +6608,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>129987</v>
+        <v>70083</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -6616,30 +6616,30 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="E76" t="n">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>44054.73262731481</v>
+        <v>43867.40498842593</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6690,7 +6690,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>27751</v>
+        <v>90445</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -6698,30 +6698,30 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="E77" t="n">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>43738.68260416666</v>
+        <v>43915.60283564815</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6772,7 +6772,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>89395</v>
+        <v>112087</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -6780,13 +6780,13 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E78" t="n">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="F78" s="2" t="n">
-        <v>43913.60846064815</v>
+        <v>43983.60597222222</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -6854,7 +6854,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>111048</v>
+        <v>132222</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -6862,13 +6862,13 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="E79" t="n">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="F79" s="2" t="n">
-        <v>43981.00342592593</v>
+        <v>44057.59260416667</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -6881,7 +6881,7 @@
         </is>
       </c>
       <c r="I79" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -6936,7 +6936,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>7029</v>
+        <v>50009</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -6944,13 +6944,13 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F80" s="2" t="n">
-        <v>43372.33032407407</v>
+        <v>43801.64949074074</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -6963,7 +6963,7 @@
         </is>
       </c>
       <c r="I80" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -7018,7 +7018,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>48928</v>
+        <v>91480</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -7026,30 +7026,30 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="E81" t="n">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="F81" s="2" t="n">
-        <v>43798.66496527778</v>
+        <v>43917.59643518519</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -7100,7 +7100,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>69122</v>
+        <v>9674</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -7108,13 +7108,13 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E82" t="n">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="F82" s="2" t="n">
-        <v>43854.62575231482</v>
+        <v>43375.77115740741</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -7127,7 +7127,7 @@
         </is>
       </c>
       <c r="I82" t="n">
-        <v>18362</v>
+        <v>17134</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -7182,7 +7182,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>131030</v>
+        <v>30149</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -7190,30 +7190,30 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="E83" t="n">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="F83" s="2" t="n">
-        <v>44055.63931712963</v>
+        <v>43742.68920138889</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -7264,7 +7264,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>28961</v>
+        <v>51172</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -7272,13 +7272,13 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E84" t="n">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="F84" s="2" t="n">
-        <v>43740.68269675926</v>
+        <v>43803.66293981481</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -7346,7 +7346,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>70083</v>
+        <v>71170</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -7354,13 +7354,13 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E85" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F85" s="2" t="n">
-        <v>43867.40498842593</v>
+        <v>43868.76869212963</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>90445</v>
+        <v>92093</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -7436,13 +7436,13 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E86" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F86" s="2" t="n">
-        <v>43915.60283564815</v>
+        <v>43920.5396412037</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -7510,7 +7510,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>112087</v>
+        <v>113375</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -7518,13 +7518,13 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E87" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F87" s="2" t="n">
-        <v>43983.60597222222</v>
+        <v>43985.61384259259</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -7592,7 +7592,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>132222</v>
+        <v>133422</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -7600,13 +7600,13 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E88" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F88" s="2" t="n">
-        <v>44057.59260416667</v>
+        <v>44060.58711805556</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -7674,7 +7674,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>50009</v>
+        <v>72058</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -7682,13 +7682,13 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E89" t="n">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="F89" s="2" t="n">
-        <v>43801.64949074074</v>
+        <v>43871.62813657407</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -7756,7 +7756,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>91480</v>
+        <v>92459</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -7764,13 +7764,13 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E90" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>43917.59643518519</v>
+        <v>43924.53144675926</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -7838,7 +7838,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>72058</v>
+        <v>31263</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -7846,13 +7846,13 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="E91" t="n">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="F91" s="2" t="n">
-        <v>43871.62813657407</v>
+        <v>43745.68821759259</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -7920,7 +7920,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>92093</v>
+        <v>52266</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -7928,30 +7928,30 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="E92" t="n">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="F92" s="2" t="n">
-        <v>43920.5396412037</v>
+        <v>43805.69142361111</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I92" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -8002,7 +8002,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>113375</v>
+        <v>93109</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -8010,13 +8010,13 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E93" t="n">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="F93" s="2" t="n">
-        <v>43985.61384259259</v>
+        <v>43927.59920138889</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -8084,7 +8084,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>133422</v>
+        <v>114576</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -8092,17 +8092,17 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E94" t="n">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="F94" s="2" t="n">
-        <v>44060.58711805556</v>
+        <v>43989.51265046297</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -8111,7 +8111,7 @@
         </is>
       </c>
       <c r="I94" t="n">
-        <v>19041</v>
+        <v>18363</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -8166,7 +8166,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>31263</v>
+        <v>134699</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -8174,30 +8174,30 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="E95" t="n">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="F95" s="2" t="n">
-        <v>43745.68821759259</v>
+        <v>44062.59583333333</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>18362</v>
+        <v>19041</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -8248,7 +8248,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>52266</v>
+        <v>11280</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -8256,13 +8256,13 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="E96" t="n">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="F96" s="2" t="n">
-        <v>43805.69142361111</v>
+        <v>43376.74490740741</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -8275,7 +8275,7 @@
         </is>
       </c>
       <c r="I96" t="n">
-        <v>18362</v>
+        <v>17134</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -8330,7 +8330,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>92459</v>
+        <v>32461</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -8338,30 +8338,30 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="E97" t="n">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="F97" s="2" t="n">
-        <v>43924.53144675926</v>
+        <v>43747.67650462963</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I97" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -8412,7 +8412,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>9674</v>
+        <v>73148</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -8420,30 +8420,30 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="F98" s="2" t="n">
-        <v>43375.77115740741</v>
+        <v>43873.64203703704</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I98" t="n">
-        <v>17134</v>
+        <v>18363</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -8494,7 +8494,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>30149</v>
+        <v>94064</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -8502,30 +8502,30 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="E99" t="n">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="F99" s="2" t="n">
-        <v>43742.68920138889</v>
+        <v>43929.60230324074</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I99" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -8576,7 +8576,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>51172</v>
+        <v>53249</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -8584,13 +8584,13 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E100" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F100" s="2" t="n">
-        <v>43803.66293981481</v>
+        <v>43808.70978009259</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -8658,7 +8658,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>71170</v>
+        <v>115589</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -8666,30 +8666,30 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="E101" t="n">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F101" s="2" t="n">
-        <v>43868.76869212963</v>
+        <v>43994.6406712963</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I101" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -8740,7 +8740,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>93109</v>
+        <v>135938</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -8748,13 +8748,13 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="E102" t="n">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="F102" s="2" t="n">
-        <v>43927.59920138889</v>
+        <v>44064.62328703704</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -8767,7 +8767,7 @@
         </is>
       </c>
       <c r="I102" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -8822,7 +8822,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>114576</v>
+        <v>12746</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -8830,13 +8830,13 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="E103" t="n">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F103" s="2" t="n">
-        <v>43989.51265046297</v>
+        <v>43379.18059027778</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -8845,15 +8845,15 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>18363</v>
+        <v>17134</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -8904,7 +8904,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>134699</v>
+        <v>33612</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -8912,30 +8912,30 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E104" t="n">
-        <v>154</v>
+        <v>46</v>
       </c>
       <c r="F104" s="2" t="n">
-        <v>44062.59583333333</v>
+        <v>43749.66354166667</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I104" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -8986,7 +8986,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>11280</v>
+        <v>54260</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -8994,13 +8994,13 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E105" t="n">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="F105" s="2" t="n">
-        <v>43376.74490740741</v>
+        <v>43810.6946875</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -9013,7 +9013,7 @@
         </is>
       </c>
       <c r="I105" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -9068,7 +9068,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>32461</v>
+        <v>74224</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -9076,30 +9076,30 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E106" t="n">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F106" s="2" t="n">
-        <v>43747.67650462963</v>
+        <v>43875.63653935185</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -9150,7 +9150,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>73148</v>
+        <v>95038</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -9158,13 +9158,13 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="E107" t="n">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="F107" s="2" t="n">
-        <v>43873.64203703704</v>
+        <v>43931.57861111111</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -9232,7 +9232,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>94064</v>
+        <v>116559</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -9240,13 +9240,13 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E108" t="n">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="F108" s="2" t="n">
-        <v>43929.60230324074</v>
+        <v>43998.69706018519</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -9314,7 +9314,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>53249</v>
+        <v>75223</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -9322,30 +9322,30 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E109" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F109" s="2" t="n">
-        <v>43808.70978009259</v>
+        <v>43878.69207175926</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I109" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -9396,7 +9396,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>115589</v>
+        <v>96012</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -9404,13 +9404,13 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E110" t="n">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="F110" s="2" t="n">
-        <v>43994.6406712963</v>
+        <v>43934.59964120371</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>135938</v>
+        <v>137017</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -9486,13 +9486,13 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E111" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F111" s="2" t="n">
-        <v>44064.62328703704</v>
+        <v>44067.59159722222</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -9560,7 +9560,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>12746</v>
+        <v>14007</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -9568,13 +9568,13 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E112" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F112" s="2" t="n">
-        <v>43379.18059027778</v>
+        <v>43381.98327546296</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -9642,7 +9642,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>33612</v>
+        <v>34790</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -9650,13 +9650,13 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E113" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F113" s="2" t="n">
-        <v>43749.66354166667</v>
+        <v>43768.65552083333</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -9724,7 +9724,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>54260</v>
+        <v>55266</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -9732,13 +9732,13 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E114" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F114" s="2" t="n">
-        <v>43810.6946875</v>
+        <v>43812.65584490741</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -9806,7 +9806,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>74224</v>
+        <v>117612</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -9814,13 +9814,13 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="E115" t="n">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="F115" s="2" t="n">
-        <v>43875.63653935185</v>
+        <v>44001.51723379629</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -9888,7 +9888,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>95038</v>
+        <v>76189</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -9896,13 +9896,13 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E116" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="F116" s="2" t="n">
-        <v>43931.57861111111</v>
+        <v>43880.63763888889</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -9970,7 +9970,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>116559</v>
+        <v>96988</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -9978,13 +9978,13 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E117" t="n">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>43998.69706018519</v>
+        <v>43936.60435185185</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -10052,7 +10052,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>75223</v>
+        <v>138305</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -10060,13 +10060,13 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="E118" t="n">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="F118" s="2" t="n">
-        <v>43878.69207175926</v>
+        <v>44069.61446759259</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -10079,7 +10079,7 @@
         </is>
       </c>
       <c r="I118" t="n">
-        <v>18363</v>
+        <v>19041</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -10134,7 +10134,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>96012</v>
+        <v>15608</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -10142,30 +10142,30 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E119" t="n">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="F119" s="2" t="n">
-        <v>43934.59964120371</v>
+        <v>43383.73309027778</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I119" t="n">
-        <v>18363</v>
+        <v>17134</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K119" t="inlineStr">
@@ -10216,7 +10216,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>137017</v>
+        <v>35848</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -10224,30 +10224,30 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="E120" t="n">
-        <v>156</v>
+        <v>48</v>
       </c>
       <c r="F120" s="2" t="n">
-        <v>44067.59159722222</v>
+        <v>43770.74552083333</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I120" t="n">
-        <v>19041</v>
+        <v>18362</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K120" t="inlineStr">
@@ -10298,7 +10298,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>14007</v>
+        <v>36216</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -10306,13 +10306,13 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E121" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="F121" s="2" t="n">
-        <v>43381.98327546296</v>
+        <v>43773.51679398148</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -10325,7 +10325,7 @@
         </is>
       </c>
       <c r="I121" t="n">
-        <v>17134</v>
+        <v>18362</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -10380,7 +10380,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>34790</v>
+        <v>56349</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -10388,13 +10388,13 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E122" t="n">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F122" s="2" t="n">
-        <v>43768.65552083333</v>
+        <v>43815.63793981481</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -10462,7 +10462,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>55266</v>
+        <v>77229</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -10470,30 +10470,30 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E123" t="n">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="F123" s="2" t="n">
-        <v>43812.65584490741</v>
+        <v>43882.60393518519</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Майкрософт Windows 10 Pro</t>
+          <t>Microsoft Windows 10 Pro</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>64-разрядная</t>
+          <t>64-bit</t>
         </is>
       </c>
       <c r="I123" t="n">
-        <v>18362</v>
+        <v>18363</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>ru-RU</t>
+          <t>ru-RU en-US</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
@@ -10544,7 +10544,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>117612</v>
+        <v>97943</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -10552,13 +10552,13 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E124" t="n">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="F124" s="2" t="n">
-        <v>44001.51723379629</v>
+        <v>43938.57678240741</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -10626,7 +10626,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>76189</v>
+        <v>118690</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E125" t="n">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>43880.63763888889</v>
+        <v>44005.76278935185</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -10708,7 +10708,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>96988</v>
+        <v>57477</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -10716,30 +10716,30 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="E126" t="n">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>43936.60435185185</v>
+        <v>43817.69225694444</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Microsoft Windows 10 Pro</t>
+          <t>Майкрософт Windows 10 Pro</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>64-bit</t>
+          <t>64-разрядная</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>18363</v>
+        <v>18362</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>ru-RU en-US</t>
+          <t>ru-RU</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -10790,7 +10790,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>138305</v>
+        <v>119680</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -10798,13 +10798,13 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E127" t="n">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F127" s="2" t="n">
-        <v>44069.61446759259</v>
+        <v>44008.61280092593</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -10817,53 +10817,135 @@
         </is>
       </c>
       <c r="I127" t="n">
+        <v>18363</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>ru-RU en-US</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>ASUSTeK COMPUTER INC.</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>B85M-G</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>Rev X.0x</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>American Megatrends Inc.</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>BIOS Date: 07/22/15 14:30:56 Ver: 25.01</t>
+        </is>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>ALASKA - 1072009</t>
+        </is>
+      </c>
+      <c r="Q127" t="n">
+        <v>4</v>
+      </c>
+      <c r="R127" t="n">
+        <v>4</v>
+      </c>
+      <c r="S127" t="n">
+        <v>8</v>
+      </c>
+      <c r="T127" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>139548</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>90514-WS404</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>131</v>
+      </c>
+      <c r="E128" t="n">
+        <v>158</v>
+      </c>
+      <c r="F128" s="2" t="n">
+        <v>44071.5894212963</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Microsoft Windows 10 Pro</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>64-bit</t>
+        </is>
+      </c>
+      <c r="I128" t="n">
         <v>19041</v>
       </c>
-      <c r="J127" t="inlineStr">
+      <c r="J128" t="inlineStr">
         <is>
           <t>ru-RU en-US</t>
         </is>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>ASUSTeK COMPUTER INC.</t>
-        </is>
-      </c>
-      <c r="L127" t="inlineStr">
-        <is>
-          <t>B85M-G</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>Rev X.0x</t>
-        </is>
-      </c>
-      <c r="N127" t="inlineStr">
-        <is>
-          <t>American Megatrends Inc.</t>
-        </is>
-      </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>BIOS Date: 07/22/15 14:30:56 Ver: 25.01</t>
-        </is>
-      </c>
-      <c r="P127" t="inlineStr">
-        <is>
-          <t>ALASKA - 1072009</t>
-        </is>
-      </c>
-      <c r="Q127" t="n">
-        <v>4</v>
-      </c>
-      <c r="R127" t="n">
-        <v>4</v>
-      </c>
-      <c r="S127" t="n">
-        <v>8</v>
-      </c>
-      <c r="T127" t="n">
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>ASUSTeK COMPUTER INC.</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>B85M-G</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>Rev X.0x</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>American Megatrends Inc.</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>BIOS Date: 07/22/15 14:30:56 Ver: 25.01</t>
+        </is>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>ALASKA - 1072009</t>
+        </is>
+      </c>
+      <c r="Q128" t="n">
+        <v>4</v>
+      </c>
+      <c r="R128" t="n">
+        <v>4</v>
+      </c>
+      <c r="S128" t="n">
+        <v>8</v>
+      </c>
+      <c r="T128" t="n">
         <v>32</v>
       </c>
     </row>

</xml_diff>